<commit_message>
enh: sanity check crit buckling
</commit_message>
<xml_diff>
--- a/wing_optimization_SSCC/loads/evolution.xlsx
+++ b/wing_optimization_SSCC/loads/evolution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\compositeoptimization\wing_optimization_SSCC\loads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C64DB31-C812-4965-80CA-1CE0B95D4E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1027140B-A9C2-4ED3-A926-121DA0F71FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18666" yWindow="2405" windowWidth="18775" windowHeight="10066" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="time" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="95">
   <si>
     <t>iteration</t>
   </si>
@@ -267,6 +267,54 @@
   <si>
     <t>minues total run time</t>
   </si>
+  <si>
+    <t>average std</t>
+  </si>
+  <si>
+    <t>Final loads</t>
+  </si>
+  <si>
+    <t>Nzz</t>
+  </si>
+  <si>
+    <t>pnxx</t>
+  </si>
+  <si>
+    <t>pnyy</t>
+  </si>
+  <si>
+    <t>pnxy</t>
+  </si>
+  <si>
+    <t>panel</t>
+  </si>
+  <si>
+    <t>(0.25,0.12)</t>
+  </si>
+  <si>
+    <t>(0.02,0.01)</t>
+  </si>
+  <si>
+    <t>(0.01,0.14)</t>
+  </si>
+  <si>
+    <t>(0.07,0.39)</t>
+  </si>
+  <si>
+    <t>(0.11,0.14)</t>
+  </si>
+  <si>
+    <t>(0.26,0.05)</t>
+  </si>
+  <si>
+    <t>(0.20,0.01)</t>
+  </si>
+  <si>
+    <t>(0.04,0.19)</t>
+  </si>
+  <si>
+    <t>(0.01,0.53)</t>
+  </si>
 </sst>
 </file>
 
@@ -327,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -338,6 +386,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9253,18 +9302,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE25C2AA-23FC-4FBB-AF98-456EBBDF3AAC}">
-  <dimension ref="A1:Z64"/>
+  <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="7" max="7" width="9" customWidth="1"/>
     <col min="13" max="13" width="3.75" customWidth="1"/>
     <col min="16" max="16" width="17.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="18" max="25" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.75" bestFit="1" customWidth="1"/>
+    <col min="19" max="25" width="3.875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="10.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10258,6 +10309,13 @@
       </c>
       <c r="M16" t="s">
         <v>20</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>79</v>
+      </c>
+      <c r="R16" s="5">
+        <f>AVERAGE(Q14:Y14)</f>
+        <v>1.0087311357031008</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -11879,6 +11937,8 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
@@ -11886,6 +11946,349 @@
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
     </row>
+    <row r="65" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>85</v>
+      </c>
+      <c r="D66" t="s">
+        <v>3</v>
+      </c>
+      <c r="E66" t="s">
+        <v>4</v>
+      </c>
+      <c r="F66" t="s">
+        <v>81</v>
+      </c>
+      <c r="G66" t="s">
+        <v>82</v>
+      </c>
+      <c r="H66" t="s">
+        <v>83</v>
+      </c>
+      <c r="I66" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="67" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C67" s="1">
+        <v>10</v>
+      </c>
+      <c r="D67" s="2">
+        <v>-2413.2969069999999</v>
+      </c>
+      <c r="E67" s="2">
+        <v>-607.77428129999998</v>
+      </c>
+      <c r="F67" s="2">
+        <v>291.44217190000001</v>
+      </c>
+      <c r="G67">
+        <f>ABS(D67/D67)</f>
+        <v>1</v>
+      </c>
+      <c r="H67" s="6">
+        <f>ABS(E67/D67)</f>
+        <v>0.25184397308805734</v>
+      </c>
+      <c r="I67" s="6">
+        <f>ABS(F67/D67)</f>
+        <v>0.1207651537009988</v>
+      </c>
+      <c r="J67" t="str">
+        <f>_xlfn.CONCAT("(",G67,",",H67,",",I67)</f>
+        <v>(1,0.251843973088057,0.120765153700999</v>
+      </c>
+    </row>
+    <row r="68" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C68" s="1">
+        <v>11</v>
+      </c>
+      <c r="D68" s="2">
+        <v>-1519.608782</v>
+      </c>
+      <c r="E68" s="2">
+        <v>-40.736502819999998</v>
+      </c>
+      <c r="F68" s="2">
+        <v>-29.929870000000001</v>
+      </c>
+      <c r="G68">
+        <f t="shared" ref="G68:G75" si="1">ABS(D68/D68)</f>
+        <v>1</v>
+      </c>
+      <c r="H68" s="6">
+        <f t="shared" ref="H68:H75" si="2">ABS(E68/D68)</f>
+        <v>2.6807230454660533E-2</v>
+      </c>
+      <c r="I68" s="6">
+        <f t="shared" ref="I68:I75" si="3">ABS(F68/D68)</f>
+        <v>1.9695773250670779E-2</v>
+      </c>
+      <c r="J68" t="str">
+        <f t="shared" ref="J68:J75" si="4">_xlfn.CONCAT("(",G68,",",H68,",",I68)</f>
+        <v>(1,0.0268072304546605,0.0196957732506708</v>
+      </c>
+    </row>
+    <row r="69" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C69" s="1">
+        <v>12</v>
+      </c>
+      <c r="D69" s="2">
+        <v>-449.3331657</v>
+      </c>
+      <c r="E69" s="2">
+        <v>2.8955858750000001</v>
+      </c>
+      <c r="F69" s="2">
+        <v>-61.942467499999999</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H69" s="6">
+        <f t="shared" si="2"/>
+        <v>6.4441846185314877E-3</v>
+      </c>
+      <c r="I69" s="6">
+        <f t="shared" si="3"/>
+        <v>0.13785420758670697</v>
+      </c>
+      <c r="J69" t="str">
+        <f t="shared" si="4"/>
+        <v>(1,0.00644418461853149,0.137854207586707</v>
+      </c>
+    </row>
+    <row r="70" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C70" s="1">
+        <v>13</v>
+      </c>
+      <c r="D70" s="2">
+        <v>-448.05270000000002</v>
+      </c>
+      <c r="E70" s="2">
+        <v>30.941809379999999</v>
+      </c>
+      <c r="F70" s="2">
+        <v>-176.95502819999999</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H70" s="6">
+        <f t="shared" si="2"/>
+        <v>6.9058415181964081E-2</v>
+      </c>
+      <c r="I70" s="6">
+        <f t="shared" si="3"/>
+        <v>0.39494244360094244</v>
+      </c>
+      <c r="J70" t="str">
+        <f t="shared" si="4"/>
+        <v>(1,0.0690584151819641,0.394942443600942</v>
+      </c>
+    </row>
+    <row r="71" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C71" s="1">
+        <v>14</v>
+      </c>
+      <c r="D71" s="2">
+        <v>-1474.017625</v>
+      </c>
+      <c r="E71" s="2">
+        <v>-155.11935</v>
+      </c>
+      <c r="F71" s="2">
+        <v>-209.19045</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H71" s="6">
+        <f t="shared" si="2"/>
+        <v>0.10523574980997938</v>
+      </c>
+      <c r="I71" s="6">
+        <f t="shared" si="3"/>
+        <v>0.14191855406070875</v>
+      </c>
+      <c r="J71" t="str">
+        <f t="shared" si="4"/>
+        <v>(1,0.105235749809979,0.141918554060709</v>
+      </c>
+    </row>
+    <row r="72" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C72" s="1">
+        <v>15</v>
+      </c>
+      <c r="D72" s="2">
+        <v>-2782.6806879999999</v>
+      </c>
+      <c r="E72" s="2">
+        <v>-715.9270563</v>
+      </c>
+      <c r="F72" s="2">
+        <v>-126.92502500000001</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H72" s="6">
+        <f t="shared" si="2"/>
+        <v>0.25727962945491933</v>
+      </c>
+      <c r="I72" s="6">
+        <f t="shared" si="3"/>
+        <v>4.5612500761352183E-2</v>
+      </c>
+      <c r="J72" t="str">
+        <f t="shared" si="4"/>
+        <v>(1,0.257279629454919,0.0456125007613522</v>
+      </c>
+    </row>
+    <row r="73" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C73" s="1">
+        <v>16</v>
+      </c>
+      <c r="D73" s="2">
+        <v>-2831.1223749999999</v>
+      </c>
+      <c r="E73" s="2">
+        <v>-585.61413440000001</v>
+      </c>
+      <c r="F73" s="2">
+        <v>22.45525632</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H73" s="6">
+        <f t="shared" si="2"/>
+        <v>0.20684875354425469</v>
+      </c>
+      <c r="I73" s="6">
+        <f t="shared" si="3"/>
+        <v>7.9315738939048867E-3</v>
+      </c>
+      <c r="J73" t="str">
+        <f t="shared" si="4"/>
+        <v>(1,0.206848753544255,0.00793157389390489</v>
+      </c>
+    </row>
+    <row r="74" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C74" s="1">
+        <v>17</v>
+      </c>
+      <c r="D74" s="2">
+        <v>-1670.3654690000001</v>
+      </c>
+      <c r="E74" s="2">
+        <v>-65.819476249999994</v>
+      </c>
+      <c r="F74" s="2">
+        <v>-324.79375320000003</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H74" s="6">
+        <f t="shared" si="2"/>
+        <v>3.9404236660498151E-2</v>
+      </c>
+      <c r="I74" s="6">
+        <f t="shared" si="3"/>
+        <v>0.19444472435989996</v>
+      </c>
+      <c r="J74" t="str">
+        <f t="shared" si="4"/>
+        <v>(1,0.0394042366604982,0.1944447243599</v>
+      </c>
+    </row>
+    <row r="75" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C75" s="1">
+        <v>18</v>
+      </c>
+      <c r="D75" s="2">
+        <v>-531.50832500000001</v>
+      </c>
+      <c r="E75" s="2">
+        <v>7.9851393750000002</v>
+      </c>
+      <c r="F75" s="2">
+        <v>-284.7068688</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H75" s="6">
+        <f t="shared" si="2"/>
+        <v>1.5023545256793485E-2</v>
+      </c>
+      <c r="I75" s="6">
+        <f t="shared" si="3"/>
+        <v>0.53565834326301476</v>
+      </c>
+      <c r="J75" t="str">
+        <f t="shared" si="4"/>
+        <v>(1,0.0150235452567935,0.535658343263015</v>
+      </c>
+    </row>
+    <row r="78" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I78" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="79" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I79" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="80" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I80" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I81" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="82" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I82" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I83" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="84" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I84" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="85" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I85" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="86" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I86" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
enh: refined FEM check write up
</commit_message>
<xml_diff>
--- a/wing_optimization_SSCC/loads/evolution.xlsx
+++ b/wing_optimization_SSCC/loads/evolution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\compositeoptimization\wing_optimization_SSCC\loads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1027140B-A9C2-4ED3-A926-121DA0F71FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9759E061-F1FD-47DD-8857-4D172489BC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18666" yWindow="2405" windowWidth="18775" windowHeight="10066" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="97">
   <si>
     <t>iteration</t>
   </si>
@@ -314,6 +314,12 @@
   </si>
   <si>
     <t>(0.01,0.53)</t>
+  </si>
+  <si>
+    <t>nev</t>
+  </si>
+  <si>
+    <t>n runs</t>
   </si>
 </sst>
 </file>
@@ -9173,10 +9179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -9295,6 +9301,12 @@
         <v>78</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f>0.7*60</f>
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9304,8 +9316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE25C2AA-23FC-4FBB-AF98-456EBBDF3AAC}">
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I77" sqref="I77"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -11925,9 +11937,23 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
+      <c r="I58" t="s">
+        <v>95</v>
+      </c>
+      <c r="J58">
+        <f>SUM(J2:J55)</f>
+        <v>3585</v>
+      </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
+      <c r="I59" t="s">
+        <v>96</v>
+      </c>
+      <c r="J59">
+        <f>J58/54</f>
+        <v>66.388888888888886</v>
+      </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>

</xml_diff>